<commit_message>
letting empty cells slide for now in parse.py
</commit_message>
<xml_diff>
--- a/data/address errors.xlsx
+++ b/data/address errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinabeshai/School/Junior/Fall/COS333i/fair-share-housing-5/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA83A23-EF1B-DA4A-823E-4F4DC6FCCED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EDC925-7060-B54E-9BAF-DCC51F28271A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27480" windowHeight="16140" xr2:uid="{129652EC-9F8C-3B42-82FF-3C73F84312CD}"/>
   </bookViews>
@@ -2017,10 +2017,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CD3CD4-8082-984A-BCC5-8BEEC687BD02}">
   <dimension ref="A1:AY159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="W1" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2188,9 +2188,6 @@
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>1426</v>
-      </c>
       <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
@@ -2334,9 +2331,6 @@
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>1426</v>
-      </c>
       <c r="B3" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>